<commit_message>
izdelava baze vendar se ne dela, tezave z vrsticami in stolpci
</commit_message>
<xml_diff>
--- a/variables_input.xlsx
+++ b/variables_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janpe\Desktop\Faks\Magisterska\raziskava\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A99C19-66A5-4BE1-947A-2441E5F64CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC22E2-4136-475C-B6C9-BBC4B879FE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-4110" windowWidth="38620" windowHeight="21220" xr2:uid="{F6274D12-767B-4A34-8136-D953A83744CB}"/>
+    <workbookView xWindow="44800" yWindow="-4000" windowWidth="19200" windowHeight="10500" xr2:uid="{F6274D12-767B-4A34-8136-D953A83744CB}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="347">
   <si>
     <t>Spremenljivka</t>
   </si>
@@ -1283,13 +1283,25 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>type_sql</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>TEXT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1319,6 +1331,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1340,7 +1359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1348,6 +1367,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
@@ -1662,10 +1682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05736F53-14C5-42D3-8B31-649468058E6D}">
-  <dimension ref="A1:DR18"/>
+  <dimension ref="A1:DR20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="CW4" sqref="CW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2881,1479 +2901,1844 @@
     </row>
     <row r="4" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
-      </c>
-      <c r="B4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1234</v>
-      </c>
-      <c r="G4">
-        <v>12334</v>
-      </c>
-      <c r="H4" t="s">
-        <v>326</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>2467</v>
-      </c>
-      <c r="K4" t="s">
-        <v>327</v>
-      </c>
-      <c r="L4" t="s">
-        <v>328</v>
-      </c>
-      <c r="M4" t="s">
-        <v>329</v>
-      </c>
-      <c r="N4" t="b">
-        <v>1</v>
-      </c>
-      <c r="O4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>330</v>
-      </c>
-      <c r="S4" t="s">
-        <v>331</v>
-      </c>
-      <c r="T4" t="s">
-        <v>332</v>
-      </c>
-      <c r="U4" t="s">
-        <v>333</v>
-      </c>
-      <c r="V4" t="s">
-        <v>334</v>
-      </c>
-      <c r="W4" t="s">
-        <v>335</v>
-      </c>
-      <c r="X4">
-        <v>360</v>
-      </c>
-      <c r="Y4">
-        <v>360</v>
-      </c>
-      <c r="Z4">
-        <v>360</v>
-      </c>
-      <c r="AA4">
-        <v>360</v>
-      </c>
-      <c r="AB4">
-        <v>360</v>
-      </c>
-      <c r="AC4">
-        <v>360</v>
-      </c>
-      <c r="AD4">
-        <v>360</v>
-      </c>
-      <c r="AE4">
-        <v>360</v>
-      </c>
-      <c r="AF4">
-        <v>360</v>
-      </c>
-      <c r="AG4">
-        <v>360</v>
-      </c>
-      <c r="AH4">
-        <v>360</v>
-      </c>
-      <c r="AI4">
-        <v>360</v>
-      </c>
-      <c r="AJ4">
-        <v>100</v>
-      </c>
-      <c r="AK4">
-        <v>100</v>
-      </c>
-      <c r="AL4">
-        <v>100</v>
-      </c>
-      <c r="AM4">
-        <v>100</v>
-      </c>
-      <c r="AN4">
-        <v>100</v>
-      </c>
-      <c r="AO4">
-        <v>100</v>
-      </c>
-      <c r="AP4">
-        <v>30</v>
-      </c>
-      <c r="AQ4">
-        <v>15</v>
-      </c>
-      <c r="AR4">
-        <v>0</v>
-      </c>
-      <c r="AS4">
-        <v>-15</v>
-      </c>
-      <c r="AT4">
-        <v>-30</v>
-      </c>
-      <c r="AU4">
-        <v>-45</v>
-      </c>
-      <c r="AV4">
-        <v>-60</v>
-      </c>
-      <c r="AW4">
-        <v>-75</v>
-      </c>
-      <c r="AX4">
-        <v>-90</v>
-      </c>
-      <c r="AY4">
-        <v>-105</v>
-      </c>
-      <c r="AZ4">
-        <v>-120</v>
-      </c>
-      <c r="BA4">
-        <v>-135</v>
-      </c>
-      <c r="BB4">
-        <v>-150</v>
-      </c>
-      <c r="BC4">
-        <v>-165</v>
-      </c>
-      <c r="BD4">
-        <v>-180</v>
-      </c>
-      <c r="BE4">
-        <v>-195</v>
-      </c>
-      <c r="BF4">
-        <v>-210</v>
-      </c>
-      <c r="BG4">
-        <v>-225</v>
-      </c>
-      <c r="BH4">
-        <v>-240</v>
-      </c>
-      <c r="BI4">
-        <v>-255</v>
-      </c>
-      <c r="BJ4">
-        <v>-270</v>
-      </c>
-      <c r="BK4">
-        <v>-285</v>
-      </c>
-      <c r="BL4">
-        <v>-300</v>
-      </c>
-      <c r="BM4">
-        <v>-315</v>
-      </c>
-      <c r="BN4">
-        <v>-330</v>
-      </c>
-      <c r="BO4">
-        <v>-345</v>
-      </c>
-      <c r="BP4">
-        <v>-360</v>
-      </c>
-      <c r="BQ4">
-        <v>-375</v>
-      </c>
-      <c r="BR4">
-        <v>-390</v>
-      </c>
-      <c r="BS4">
-        <v>-405</v>
-      </c>
-      <c r="BT4">
-        <v>-420</v>
-      </c>
-      <c r="BU4">
-        <v>-435</v>
-      </c>
-      <c r="BV4">
-        <v>-450</v>
-      </c>
-      <c r="BW4">
-        <v>-465</v>
-      </c>
-      <c r="BX4">
-        <v>-480</v>
-      </c>
-      <c r="BY4">
-        <v>-495</v>
-      </c>
-      <c r="BZ4">
-        <v>-510</v>
-      </c>
-      <c r="CA4">
-        <v>-525</v>
-      </c>
-      <c r="CB4">
-        <v>-540</v>
-      </c>
-      <c r="CC4">
-        <v>-555</v>
-      </c>
-      <c r="CD4">
-        <v>-570</v>
-      </c>
-      <c r="CE4">
-        <v>-585</v>
-      </c>
-      <c r="CF4">
-        <v>-600</v>
-      </c>
-      <c r="CG4">
-        <v>-615</v>
-      </c>
-      <c r="CH4">
-        <v>-630</v>
-      </c>
-      <c r="CI4">
-        <v>-645</v>
-      </c>
-      <c r="CJ4">
-        <v>-660</v>
-      </c>
-      <c r="CK4">
-        <v>-675</v>
-      </c>
-      <c r="CL4">
-        <v>-690</v>
-      </c>
-      <c r="CM4">
-        <v>-705</v>
-      </c>
-      <c r="CN4">
-        <v>-720</v>
-      </c>
-      <c r="CO4">
-        <v>-735</v>
-      </c>
-      <c r="CP4">
-        <v>-750</v>
-      </c>
-      <c r="CQ4">
-        <v>-765</v>
-      </c>
-      <c r="CR4">
-        <v>-780</v>
-      </c>
-      <c r="CS4">
-        <v>-795</v>
-      </c>
-      <c r="CT4">
-        <v>0</v>
-      </c>
-      <c r="CU4">
-        <v>0</v>
-      </c>
-      <c r="CV4" t="s">
-        <v>336</v>
-      </c>
-      <c r="CW4" t="s">
-        <v>337</v>
-      </c>
-      <c r="CX4" t="b">
-        <v>1</v>
-      </c>
-      <c r="CY4">
-        <v>657</v>
-      </c>
-      <c r="CZ4">
-        <v>567</v>
-      </c>
-      <c r="DA4">
-        <v>45</v>
-      </c>
-      <c r="DB4">
-        <v>14</v>
-      </c>
-      <c r="DC4">
-        <v>14</v>
-      </c>
-      <c r="DD4">
-        <v>14</v>
-      </c>
-      <c r="DE4">
-        <v>14</v>
-      </c>
-      <c r="DF4">
-        <v>14</v>
-      </c>
-      <c r="DG4">
-        <v>14</v>
-      </c>
-      <c r="DH4">
-        <v>456466</v>
-      </c>
-      <c r="DI4">
-        <v>56</v>
-      </c>
-      <c r="DJ4">
-        <v>6</v>
-      </c>
-      <c r="DK4">
-        <v>-44</v>
-      </c>
-      <c r="DL4">
-        <v>-94</v>
-      </c>
-      <c r="DM4">
-        <v>-144</v>
-      </c>
-      <c r="DN4">
-        <v>-194</v>
-      </c>
-      <c r="DO4">
-        <v>-244</v>
-      </c>
-      <c r="DP4">
-        <v>-294</v>
-      </c>
-      <c r="DQ4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DR4" t="b">
-        <v>1</v>
+        <v>343</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AL4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AN4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AO4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AP4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AQ4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AR4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AS4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AT4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AU4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AV4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AW4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AX4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AY4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="AZ4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BA4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BB4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BC4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BD4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BE4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BF4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BG4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BH4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BI4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BJ4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BK4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BL4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BM4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BN4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BO4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BP4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BQ4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BR4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BS4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BT4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BU4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BV4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BW4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BX4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BY4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="BZ4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CA4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CB4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CC4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CD4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CE4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CF4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CG4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CH4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CI4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CJ4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CK4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CL4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CM4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CN4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CO4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CP4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CQ4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CR4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CS4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CT4" t="s">
+        <v>344</v>
+      </c>
+      <c r="CU4" t="s">
+        <v>344</v>
+      </c>
+      <c r="CV4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="CW4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="CX4" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="CY4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="CZ4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DA4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DB4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DC4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DD4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DE4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DF4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DG4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DH4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DI4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DJ4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DK4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DL4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DM4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DN4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DO4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DP4" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DQ4" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="DR4" s="5" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:122" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>341</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>342</v>
-      </c>
-      <c r="C5" t="s">
-        <v>342</v>
-      </c>
-      <c r="D5" t="s">
-        <v>342</v>
-      </c>
-      <c r="E5" t="s">
-        <v>342</v>
-      </c>
-      <c r="F5" t="s">
-        <v>342</v>
-      </c>
-      <c r="G5" t="s">
-        <v>342</v>
+        <v>325</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1234</v>
+      </c>
+      <c r="G5">
+        <v>12334</v>
       </c>
       <c r="H5" t="s">
-        <v>342</v>
-      </c>
-      <c r="I5" t="s">
-        <v>342</v>
-      </c>
-      <c r="J5" t="s">
-        <v>342</v>
+        <v>326</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>2467</v>
       </c>
       <c r="K5" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="L5" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="M5" t="s">
-        <v>342</v>
-      </c>
-      <c r="N5" t="s">
-        <v>342</v>
-      </c>
-      <c r="O5" t="s">
-        <v>342</v>
-      </c>
-      <c r="P5" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>342</v>
+        <v>329</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="S5" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="T5" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="U5" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="V5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="W5" t="s">
-        <v>342</v>
-      </c>
-      <c r="X5" t="s">
-        <v>342</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>342</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BF5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BG5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BH5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BI5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BJ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BK5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BL5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BM5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BN5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BO5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BP5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BQ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BR5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BS5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BT5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BU5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BV5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BW5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BY5" t="s">
-        <v>342</v>
-      </c>
-      <c r="BZ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CA5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CB5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CC5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CD5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CE5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CF5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CG5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CH5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CI5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CJ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CK5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CL5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CM5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CN5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CO5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CP5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CQ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CR5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CS5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CT5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CU5" t="s">
-        <v>342</v>
+        <v>335</v>
+      </c>
+      <c r="X5">
+        <v>360</v>
+      </c>
+      <c r="Y5">
+        <v>360</v>
+      </c>
+      <c r="Z5">
+        <v>360</v>
+      </c>
+      <c r="AA5">
+        <v>360</v>
+      </c>
+      <c r="AB5">
+        <v>360</v>
+      </c>
+      <c r="AC5">
+        <v>360</v>
+      </c>
+      <c r="AD5">
+        <v>360</v>
+      </c>
+      <c r="AE5">
+        <v>360</v>
+      </c>
+      <c r="AF5">
+        <v>360</v>
+      </c>
+      <c r="AG5">
+        <v>360</v>
+      </c>
+      <c r="AH5">
+        <v>360</v>
+      </c>
+      <c r="AI5">
+        <v>360</v>
+      </c>
+      <c r="AJ5">
+        <v>100</v>
+      </c>
+      <c r="AK5">
+        <v>100</v>
+      </c>
+      <c r="AL5">
+        <v>100</v>
+      </c>
+      <c r="AM5">
+        <v>100</v>
+      </c>
+      <c r="AN5">
+        <v>100</v>
+      </c>
+      <c r="AO5">
+        <v>100</v>
+      </c>
+      <c r="AP5">
+        <v>30</v>
+      </c>
+      <c r="AQ5">
+        <v>15</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>-15</v>
+      </c>
+      <c r="AT5">
+        <v>-30</v>
+      </c>
+      <c r="AU5">
+        <v>-45</v>
+      </c>
+      <c r="AV5">
+        <v>-60</v>
+      </c>
+      <c r="AW5">
+        <v>-75</v>
+      </c>
+      <c r="AX5">
+        <v>-90</v>
+      </c>
+      <c r="AY5">
+        <v>-105</v>
+      </c>
+      <c r="AZ5">
+        <v>-120</v>
+      </c>
+      <c r="BA5">
+        <v>-135</v>
+      </c>
+      <c r="BB5">
+        <v>-150</v>
+      </c>
+      <c r="BC5">
+        <v>-165</v>
+      </c>
+      <c r="BD5">
+        <v>-180</v>
+      </c>
+      <c r="BE5">
+        <v>-195</v>
+      </c>
+      <c r="BF5">
+        <v>-210</v>
+      </c>
+      <c r="BG5">
+        <v>-225</v>
+      </c>
+      <c r="BH5">
+        <v>-240</v>
+      </c>
+      <c r="BI5">
+        <v>-255</v>
+      </c>
+      <c r="BJ5">
+        <v>-270</v>
+      </c>
+      <c r="BK5">
+        <v>-285</v>
+      </c>
+      <c r="BL5">
+        <v>-300</v>
+      </c>
+      <c r="BM5">
+        <v>-315</v>
+      </c>
+      <c r="BN5">
+        <v>-330</v>
+      </c>
+      <c r="BO5">
+        <v>-345</v>
+      </c>
+      <c r="BP5">
+        <v>-360</v>
+      </c>
+      <c r="BQ5">
+        <v>-375</v>
+      </c>
+      <c r="BR5">
+        <v>-390</v>
+      </c>
+      <c r="BS5">
+        <v>-405</v>
+      </c>
+      <c r="BT5">
+        <v>-420</v>
+      </c>
+      <c r="BU5">
+        <v>-435</v>
+      </c>
+      <c r="BV5">
+        <v>-450</v>
+      </c>
+      <c r="BW5">
+        <v>-465</v>
+      </c>
+      <c r="BX5">
+        <v>-480</v>
+      </c>
+      <c r="BY5">
+        <v>-495</v>
+      </c>
+      <c r="BZ5">
+        <v>-510</v>
+      </c>
+      <c r="CA5">
+        <v>-525</v>
+      </c>
+      <c r="CB5">
+        <v>-540</v>
+      </c>
+      <c r="CC5">
+        <v>-555</v>
+      </c>
+      <c r="CD5">
+        <v>-570</v>
+      </c>
+      <c r="CE5">
+        <v>-585</v>
+      </c>
+      <c r="CF5">
+        <v>-600</v>
+      </c>
+      <c r="CG5">
+        <v>-615</v>
+      </c>
+      <c r="CH5">
+        <v>-630</v>
+      </c>
+      <c r="CI5">
+        <v>-645</v>
+      </c>
+      <c r="CJ5">
+        <v>-660</v>
+      </c>
+      <c r="CK5">
+        <v>-675</v>
+      </c>
+      <c r="CL5">
+        <v>-690</v>
+      </c>
+      <c r="CM5">
+        <v>-705</v>
+      </c>
+      <c r="CN5">
+        <v>-720</v>
+      </c>
+      <c r="CO5">
+        <v>-735</v>
+      </c>
+      <c r="CP5">
+        <v>-750</v>
+      </c>
+      <c r="CQ5">
+        <v>-765</v>
+      </c>
+      <c r="CR5">
+        <v>-780</v>
+      </c>
+      <c r="CS5">
+        <v>-795</v>
+      </c>
+      <c r="CT5">
+        <v>0</v>
+      </c>
+      <c r="CU5">
+        <v>0</v>
       </c>
       <c r="CV5" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="CW5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CX5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CY5" t="s">
-        <v>342</v>
-      </c>
-      <c r="CZ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DA5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DB5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DC5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DD5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DE5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DF5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DG5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DH5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DI5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DJ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DK5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DL5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DM5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DN5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DO5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DP5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DQ5" t="s">
-        <v>342</v>
-      </c>
-      <c r="DR5" t="s">
-        <v>342</v>
+        <v>337</v>
+      </c>
+      <c r="CX5" t="b">
+        <v>1</v>
+      </c>
+      <c r="CY5">
+        <v>657</v>
+      </c>
+      <c r="CZ5">
+        <v>567</v>
+      </c>
+      <c r="DA5">
+        <v>45</v>
+      </c>
+      <c r="DB5">
+        <v>14</v>
+      </c>
+      <c r="DC5">
+        <v>14</v>
+      </c>
+      <c r="DD5">
+        <v>14</v>
+      </c>
+      <c r="DE5">
+        <v>14</v>
+      </c>
+      <c r="DF5">
+        <v>14</v>
+      </c>
+      <c r="DG5">
+        <v>14</v>
+      </c>
+      <c r="DH5">
+        <v>456466</v>
+      </c>
+      <c r="DI5">
+        <v>56</v>
+      </c>
+      <c r="DJ5">
+        <v>6</v>
+      </c>
+      <c r="DK5">
+        <v>-44</v>
+      </c>
+      <c r="DL5">
+        <v>-94</v>
+      </c>
+      <c r="DM5">
+        <v>-144</v>
+      </c>
+      <c r="DN5">
+        <v>-194</v>
+      </c>
+      <c r="DO5">
+        <v>-244</v>
+      </c>
+      <c r="DP5">
+        <v>-294</v>
+      </c>
+      <c r="DQ5" t="b">
+        <v>1</v>
+      </c>
+      <c r="DR5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:122" x14ac:dyDescent="0.25">
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" t="b">
-        <v>1</v>
-      </c>
-      <c r="S6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6" t="b">
-        <v>1</v>
-      </c>
-      <c r="U6" t="b">
-        <v>1</v>
-      </c>
-      <c r="V6" t="b">
-        <v>1</v>
-      </c>
-      <c r="W6" t="b">
-        <v>1</v>
-      </c>
-      <c r="X6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AH6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AJ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AK6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AO6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AR6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AS6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AT6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AU6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AV6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AW6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AY6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BA6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BE6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BF6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BH6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BI6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BJ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BK6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BL6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BM6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BN6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BP6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BQ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BR6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BS6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BT6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BU6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BV6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BW6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BX6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BY6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BZ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CA6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CB6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CC6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CD6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CE6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CF6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CG6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CH6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CI6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CJ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CK6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CL6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CM6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CN6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CO6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CP6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CQ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CR6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CS6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CT6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CU6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CV6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CW6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CX6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CY6" t="b">
-        <v>1</v>
-      </c>
-      <c r="CZ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DA6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DB6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DC6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DD6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DE6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DF6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DG6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DH6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DI6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DJ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DK6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DL6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DM6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DN6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DO6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DP6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DQ6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DR6" t="b">
-        <v>1</v>
+      <c r="A6" t="s">
+        <v>341</v>
+      </c>
+      <c r="B6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C6" t="s">
+        <v>342</v>
+      </c>
+      <c r="D6" t="s">
+        <v>342</v>
+      </c>
+      <c r="E6" t="s">
+        <v>342</v>
+      </c>
+      <c r="F6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G6" t="s">
+        <v>342</v>
+      </c>
+      <c r="H6" t="s">
+        <v>342</v>
+      </c>
+      <c r="I6" t="s">
+        <v>342</v>
+      </c>
+      <c r="J6" t="s">
+        <v>342</v>
+      </c>
+      <c r="K6" t="s">
+        <v>342</v>
+      </c>
+      <c r="L6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M6" t="s">
+        <v>342</v>
+      </c>
+      <c r="N6" t="s">
+        <v>342</v>
+      </c>
+      <c r="O6" t="s">
+        <v>342</v>
+      </c>
+      <c r="P6" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>342</v>
+      </c>
+      <c r="R6" t="s">
+        <v>342</v>
+      </c>
+      <c r="S6" t="s">
+        <v>342</v>
+      </c>
+      <c r="T6" t="s">
+        <v>342</v>
+      </c>
+      <c r="U6" t="s">
+        <v>342</v>
+      </c>
+      <c r="V6" t="s">
+        <v>342</v>
+      </c>
+      <c r="W6" t="s">
+        <v>342</v>
+      </c>
+      <c r="X6" t="s">
+        <v>342</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>342</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BN6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BO6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BP6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BQ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BR6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BS6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BT6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BU6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BV6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BW6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BX6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BY6" t="s">
+        <v>342</v>
+      </c>
+      <c r="BZ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CA6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CB6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CC6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CD6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CE6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CF6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CG6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CH6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CI6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CJ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CK6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CL6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CM6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CN6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CO6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CP6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CQ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CR6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CS6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CT6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CU6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CV6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CW6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CX6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CY6" t="s">
+        <v>342</v>
+      </c>
+      <c r="CZ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DA6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DB6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DC6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DD6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DE6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DF6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DG6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DH6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DI6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DJ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DK6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DL6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DM6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DN6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DO6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DP6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DQ6" t="s">
+        <v>342</v>
+      </c>
+      <c r="DR6" t="s">
+        <v>342</v>
       </c>
     </row>
-    <row r="8" spans="1:122" ht="165" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="7" spans="1:122" x14ac:dyDescent="0.25">
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7" t="b">
+        <v>1</v>
+      </c>
+      <c r="U7" t="b">
+        <v>1</v>
+      </c>
+      <c r="V7" t="b">
+        <v>1</v>
+      </c>
+      <c r="W7" t="b">
+        <v>1</v>
+      </c>
+      <c r="X7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AW7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AZ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BE7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BF7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BH7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BI7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BJ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BK7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BL7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BM7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BN7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BP7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BQ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BR7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BS7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BT7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BU7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BV7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BW7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BX7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BY7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BZ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CA7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CB7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CC7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CD7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CE7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CF7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CG7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CH7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CI7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CJ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CK7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CL7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CM7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CN7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CO7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CP7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CQ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CR7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CS7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CU7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CV7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CW7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CX7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CY7" t="b">
+        <v>1</v>
+      </c>
+      <c r="CZ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DA7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DB7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DC7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DD7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DE7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DF7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DG7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DH7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DI7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DJ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DK7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DL7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DM7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DN7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DO7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DP7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DQ7" t="b">
+        <v>1</v>
+      </c>
+      <c r="DR7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:122" ht="165" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>204</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>205</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>206</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>207</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E10" t="s">
         <v>208</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F10" t="s">
         <v>209</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G10" t="s">
         <v>210</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H10" t="s">
         <v>211</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I10" t="s">
         <v>212</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J10" t="s">
         <v>213</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K10" t="s">
         <v>214</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L10" t="s">
         <v>215</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M10" t="s">
         <v>216</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N10" t="s">
         <v>217</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O10" t="s">
         <v>218</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="Y10" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="Z10" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AA10" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AB10" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AC10" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AD10" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="AE8" s="1" t="s">
+      <c r="AE10" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="AF8" s="1" t="s">
+      <c r="AF10" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AG10" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AH8" s="1" t="s">
+      <c r="AH10" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="AI8" s="1" t="s">
+      <c r="AI10" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="AJ8" s="1" t="s">
+      <c r="AJ10" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="AK8" s="1" t="s">
+      <c r="AK10" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="AL8" s="1" t="s">
+      <c r="AL10" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="AM8" s="1" t="s">
+      <c r="AM10" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="AN8" s="1" t="s">
+      <c r="AN10" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="AO8" s="1" t="s">
+      <c r="AO10" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="AP8" s="1" t="s">
+      <c r="AP10" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="AQ8" s="1" t="s">
+      <c r="AQ10" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="AR8" s="1" t="s">
+      <c r="AR10" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="AS8" s="1" t="s">
+      <c r="AS10" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="AT8" s="1" t="s">
+      <c r="AT10" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="AU8" s="1" t="s">
+      <c r="AU10" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="AV8" s="1" t="s">
+      <c r="AV10" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="AW8" s="1" t="s">
+      <c r="AW10" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="AX8" s="1" t="s">
+      <c r="AX10" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="AY8" s="1" t="s">
+      <c r="AY10" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="AZ8" s="1" t="s">
+      <c r="AZ10" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="BA8" s="1" t="s">
+      <c r="BA10" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="BB8" s="1" t="s">
+      <c r="BB10" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="BC8" s="1" t="s">
+      <c r="BC10" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="BD8" s="1" t="s">
+      <c r="BD10" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="BE8" s="1" t="s">
+      <c r="BE10" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="BF8" s="1" t="s">
+      <c r="BF10" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="BG8" s="1" t="s">
+      <c r="BG10" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="BH8" s="1" t="s">
+      <c r="BH10" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="BI8" s="1" t="s">
+      <c r="BI10" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="BJ8" s="1" t="s">
+      <c r="BJ10" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="BK8" s="1" t="s">
+      <c r="BK10" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="BL8" s="1" t="s">
+      <c r="BL10" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="BM8" s="1" t="s">
+      <c r="BM10" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="BN8" s="1" t="s">
+      <c r="BN10" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="BO8" s="1" t="s">
+      <c r="BO10" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="BP8" s="1" t="s">
+      <c r="BP10" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="BQ8" s="1" t="s">
+      <c r="BQ10" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="BR8" s="1" t="s">
+      <c r="BR10" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="BS8" s="1" t="s">
+      <c r="BS10" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="BT8" s="1" t="s">
+      <c r="BT10" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="BU8" s="1" t="s">
+      <c r="BU10" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="BV8" s="1" t="s">
+      <c r="BV10" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="BW8" s="1" t="s">
+      <c r="BW10" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="BX8" s="1" t="s">
+      <c r="BX10" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="BY8" s="1" t="s">
+      <c r="BY10" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="BZ8" s="1" t="s">
+      <c r="BZ10" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="CA8" s="1" t="s">
+      <c r="CA10" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="CB8" s="1" t="s">
+      <c r="CB10" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="CC8" s="1" t="s">
+      <c r="CC10" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="CD8" s="1" t="s">
+      <c r="CD10" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="CE8" s="1" t="s">
+      <c r="CE10" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="CF8" s="1" t="s">
+      <c r="CF10" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="CG8" s="1" t="s">
+      <c r="CG10" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="CH8" s="1" t="s">
+      <c r="CH10" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="CI8" s="1" t="s">
+      <c r="CI10" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="CJ8" s="1" t="s">
+      <c r="CJ10" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="CK8" s="1" t="s">
+      <c r="CK10" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="CL8" s="1" t="s">
+      <c r="CL10" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="CM8" s="1" t="s">
+      <c r="CM10" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="CN8" s="1" t="s">
+      <c r="CN10" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="CO8" s="1" t="s">
+      <c r="CO10" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="CP8" s="1" t="s">
+      <c r="CP10" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="CQ8" s="1" t="s">
+      <c r="CQ10" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="CR8" s="1" t="s">
+      <c r="CR10" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="CS8" s="1" t="s">
+      <c r="CS10" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="CT8" s="1" t="s">
+      <c r="CT10" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="CU8" s="1" t="s">
+      <c r="CU10" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="CV8" s="1" t="s">
+      <c r="CV10" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="CW8" s="1" t="s">
+      <c r="CW10" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="CY8" s="1" t="s">
+      <c r="CY10" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="CZ8" s="1" t="s">
+      <c r="CZ10" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="DA8" s="1" t="s">
+      <c r="DA10" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="DB8" s="1" t="s">
+      <c r="DB10" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="DC8" s="1" t="s">
+      <c r="DC10" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="DD8" s="1" t="s">
+      <c r="DD10" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="DE8" s="1" t="s">
+      <c r="DE10" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="DF8" s="1" t="s">
+      <c r="DF10" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="DG8" s="1" t="s">
+      <c r="DG10" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="DH8" s="1" t="s">
+      <c r="DH10" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="DI8" s="1" t="s">
+      <c r="DI10" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="DJ8" s="1" t="s">
+      <c r="DJ10" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="DK8" s="1" t="s">
+      <c r="DK10" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="DL8" s="1" t="s">
+      <c r="DL10" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="DM8" s="1" t="s">
+      <c r="DM10" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="DN8" s="1" t="s">
+      <c r="DN10" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="DO8" s="1" t="s">
+      <c r="DO10" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="DP8" s="1" t="s">
+      <c r="DP10" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="DQ8" s="1" t="s">
+      <c r="DQ10" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="DR8" s="1" t="s">
+      <c r="DR10" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="1:122" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="str">
+    <row r="16" spans="1:122" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="str">
         <f>_xlfn.TEXTJOIN(",,",FALSE,B1:DR1)</f>
         <v>current_logged_user_level,,robot_running,,robot_playback,,robot_energy_saving,,product_code,,serial_number,,alarm,,alarm_axes,,alarm_code,,alarm_date,,alarm_job,,alarm_mode,,alarm_active,,error_active,,reset_alarm,,reset_error,,axis_name_1,,axis_name_2,,axis_name_3,,axis_name_4,,axis_name_5,,axis_name_6,,axis_position_1,,axis_position_2,,axis_position_3,,axis_position_4,,axis_position_5,,axis_position_6,,axis_degree_1,,axis_degree_2,,axis_degree_3,,axis_degree_4,,axis_degree_5,,axis_degree_6,,axis_speed_1,,axis_speed_2,,axis_speed_3,,axis_speed_4,,axis_speed_5,,axis_speed_6,,speed_reducer_design_lifetime_1,,speed_reducer_design_lifetime_2,,speed_reducer_design_lifetime_3,,speed_reducer_design_lifetime_4,,speed_reducer_design_lifetime_5,,speed_reducer_design_lifetime_6,,speed_reducer_remaining_lifetime_1,,speed_reducer_remaining_lifetime_2,,speed_reducer_remaining_lifetime_3,,speed_reducer_remaining_lifetime_4,,speed_reducer_remaining_lifetime_5,,speed_reducer_remaining_lifetime_6,,amplifiers_designed_lifetime_1,,amplifiers_designed_lifetime_2,,amplifiers_designed_lifetime_3,,amplifiers_designed_lifetime_4,,amplifiers_designed_lifetime_5,,amplifiers_designed_lifetime_6,,amplifiers_remaining_lifetime_1,,amplifiers_remaining_lifetime_2,,amplifiers_remaining_lifetime_3,,amplifiers_remaining_lifetime_4,,amplifiers_remaining_lifetime_5,,amplifiers_remaining_lifetime_6,,capacitors_design_lifetime_1,,capacitors_design_lifetime_2,,capacitors_design_lifetime_3,,capacitors_design_lifetime_4,,capacitors_design_lifetime_5,,capacitors_design_lifetime_6,,capacitors_remaining_lifetime_1,,capacitors_remaining_lifetime_2,,capacitors_remaining_lifetime_3,,capacitors_remaining_lifetime_4,,capacitors_remaining_lifetime_5,,capacitors_remaining_lifetime_6,,contactors_design_lifetime_1,,contactors_design_lifetime_2,,contactors_design_lifetime_3,,contactors_design_lifetime_4,,contactors_design_lifetime_5,,contactors_design_lifetime_6,,contactors_remaining_lifetime_1,,contactors_remaining_lifetime_2,,contactors_remaining_lifetime_3,,contactors_remaining_lifetime_4,,contactors_remaining_lifetime_5,,contactors_remaining_lifetime_6,,cps_fan_designed_lifetime,,cps_fan_remaining_lifetime,,controller_box_fan_designed_lifetime,,controller_box_fan_remaining_lifetime,,regenerative_fan_designed_lifetime,,regenerative_box_fan_remaining_lifetime,,manipulator_fan_designed_lifetime,,manipulator_box_fan_remaining_lifetime,,set_job,,flange_load,,device_manufacturer,,device_model ,,device_moving,,total_moving_time,,total_playback_time,,total_servo_on_time,,encoder_temperature_1,,encoder_temperature_2,,encoder_temperature_3,,encoder_temperature_4,,encoder_temperature_5,,encoder_temperature_6,,device_serial_number,,grease_supply_design_lifetime,,grease_supply_remaining_lifetime,,wire_harness_design_lifetime,,wire_harness_remaining_lifetime,,battery_exchange_design_lifetime,,battery_exchange_remaining_lifetime,,overhaul_design_lifetime,,overhaul_remaining_lifetime,,emergency_stop,,protective_stop</v>
       </c>
     </row>
-    <row r="16" spans="1:122" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="18" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="20" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>